<commit_message>
succesfully implemented xlsx file extension
</commit_message>
<xml_diff>
--- a/document_loader/src/test.xlsx
+++ b/document_loader/src/test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyhwa\github\capstone-kyndryl\document_loader\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDEC229E-8ACF-44A7-8EB6-22B1BAF642D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F14760D-FA5E-4A51-9090-ABA03007686F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{37CCB0B9-2A36-4734-9505-25BB1D2209D4}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" activeTab="1" xr2:uid="{37CCB0B9-2A36-4734-9505-25BB1D2209D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Test1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,6 +48,18 @@
   </si>
   <si>
     <t>Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -413,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB902701-2D89-4F0D-83E6-C8CEFE5B29FD}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B22"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
@@ -665,4 +678,262 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C046EF-303A-4862-BAE9-26ECAE56392B}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>97</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>96</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>94</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>93</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>92</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>91</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>90</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>89</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>88</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>87</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>86</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>85</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>84</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>83</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>82</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>81</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>80</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>